<commit_message>
Updated and finalized the texts and questions
</commit_message>
<xml_diff>
--- a/questionnaire/Questionnaire.xlsx
+++ b/questionnaire/Questionnaire.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luba/Documents/GitHub/ba-emotional-city/InterMind/questionaire/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luba/Documents/GitHub/ba-emotional-city/InterMind/questionnaire/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F74BF9-4494-7B42-96D2-C6AC769FB23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7364A74-5CD7-6F46-B784-A7E51043E50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="3" xr2:uid="{93F42349-A365-BB45-A979-EAC45E51E427}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{93F42349-A365-BB45-A979-EAC45E51E427}"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="8" r:id="rId1"/>
@@ -422,7 +422,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="940">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="944">
   <si>
     <t>type</t>
   </si>
@@ -3369,12 +3369,24 @@
   <si>
     <t>monthly_household_income_unknown</t>
   </si>
+  <si>
+    <t>majority_comparison_alone</t>
+  </si>
+  <si>
+    <t>Ich bin allein hier</t>
+  </si>
+  <si>
+    <t>Je suis seul·e ici</t>
+  </si>
+  <si>
+    <t>I am alone here</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3401,12 +3413,6 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -3494,18 +3500,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
           <xfpb:xfComplement i="0"/>
@@ -3515,7 +3521,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4097,9 +4103,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7D6A86-C761-A748-8929-C6382F8DC5F2}">
   <dimension ref="A1:AB38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4567,7 +4573,7 @@
         <v>180</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>362</v>
@@ -4615,7 +4621,7 @@
         <v>385</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>362</v>
@@ -5912,7 +5918,9 @@
       <c r="Q36" s="8" t="s">
         <v>528</v>
       </c>
-      <c r="R36" s="8"/>
+      <c r="R36" s="8" t="s">
+        <v>940</v>
+      </c>
       <c r="S36" s="8"/>
       <c r="T36" s="8"/>
       <c r="U36" s="8"/>
@@ -6006,6 +6014,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
@@ -6049,10 +6058,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E17000D-7A8B-2F49-B31C-630698EC38C8}">
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -7448,6 +7457,9 @@
       <c r="L36" s="3" t="s">
         <v>908</v>
       </c>
+      <c r="M36" s="3" t="s">
+        <v>941</v>
+      </c>
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
       <c r="S36" s="4"/>
@@ -7905,8 +7917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFCFB3F-18A0-5B4C-9A36-4B24B146669B}">
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="112" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A99"/>
+    <sheetView topLeftCell="A16" zoomScale="112" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -8032,7 +8044,7 @@
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
     </row>
-    <row r="3" spans="1:26" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="str">
         <f>IF(base!A3 &lt;&gt; "",base!A3, "")</f>
         <v>about_this_study</v>
@@ -8350,7 +8362,7 @@
       <c r="Y10" s="4"/>
       <c r="Z10" s="4"/>
     </row>
-    <row r="11" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="str">
         <f>IF(base!A11 &lt;&gt; "",base!A11, "")</f>
         <v>sexual_orientation</v>
@@ -8446,7 +8458,7 @@
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
     </row>
-    <row r="13" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="str">
         <f>IF(base!A13 &lt;&gt; "",base!A13, "")</f>
         <v>household_members</v>
@@ -8501,7 +8513,7 @@
       <c r="Y13" s="4"/>
       <c r="Z13" s="4"/>
     </row>
-    <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="str">
         <f>IF(base!A14 &lt;&gt; "",base!A14, "")</f>
         <v>household_members_financing</v>
@@ -8607,7 +8619,7 @@
       <c r="Y15" s="4"/>
       <c r="Z15" s="4"/>
     </row>
-    <row r="16" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="str">
         <f>IF(base!A16 &lt;&gt; "",base!A16, "")</f>
         <v>employment_status</v>
@@ -8691,7 +8703,7 @@
       <c r="Y17" s="4"/>
       <c r="Z17" s="4"/>
     </row>
-    <row r="18" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="str">
         <f>IF(base!A18 &lt;&gt; "",base!A18, "")</f>
         <v>different_country_than_born_in</v>
@@ -8787,7 +8799,7 @@
       <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
     </row>
-    <row r="20" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="str">
         <f>IF(base!A20 &lt;&gt; "",base!A20, "")</f>
         <v>info_current_location</v>
@@ -8822,7 +8834,7 @@
       <c r="Y20" s="4"/>
       <c r="Z20" s="4"/>
     </row>
-    <row r="21" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="str">
         <f>IF(base!A21 &lt;&gt; "",base!A21, "")</f>
         <v>indoors_outdoors</v>
@@ -9034,7 +9046,7 @@
       <c r="Y24" s="4"/>
       <c r="Z24" s="4"/>
     </row>
-    <row r="25" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="str">
         <f>IF(base!A25 &lt;&gt; "",base!A25, "")</f>
         <v>environment_noise</v>
@@ -9073,7 +9085,7 @@
       </c>
       <c r="Z25" s="4"/>
     </row>
-    <row r="26" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="str">
         <f>IF(base!A26 &lt;&gt; "",base!A26, "")</f>
         <v>environment_nature</v>
@@ -9112,7 +9124,7 @@
       </c>
       <c r="Z26" s="4"/>
     </row>
-    <row r="27" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="str">
         <f>IF(base!A27 &lt;&gt; "",base!A27, "")</f>
         <v>environment_lively</v>
@@ -9151,7 +9163,7 @@
       </c>
       <c r="Z27" s="4"/>
     </row>
-    <row r="28" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="str">
         <f>IF(base!A28 &lt;&gt; "",base!A28, "")</f>
         <v>environmen_pleasure</v>
@@ -9225,7 +9237,7 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="4"/>
     </row>
-    <row r="30" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="str">
         <f>IF(base!A30 &lt;&gt; "",base!A30, "")</f>
         <v>general_wellbeing</v>
@@ -9381,7 +9393,7 @@
       </c>
       <c r="Z33" s="4"/>
     </row>
-    <row r="34" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="str">
         <f>IF(base!A34 &lt;&gt; "",base!A34, "")</f>
         <v>sense_of_belonging</v>
@@ -9515,7 +9527,9 @@
       <c r="L36" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="M36" s="3"/>
+      <c r="M36" s="3" t="s">
+        <v>943</v>
+      </c>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
@@ -9530,7 +9544,7 @@
       <c r="Y36" s="4"/>
       <c r="Z36" s="4"/>
     </row>
-    <row r="37" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="str">
         <f>IF(base!A37 &lt;&gt; "",base!A37, "")</f>
         <v>other_factors_negative</v>
@@ -9565,7 +9579,7 @@
       <c r="Y37" s="4"/>
       <c r="Z37" s="4"/>
     </row>
-    <row r="38" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="str">
         <f>IF(base!A38 &lt;&gt; "",base!A38, "")</f>
         <v>other_factors_positive</v>
@@ -9968,6 +9982,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -9976,8 +9991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5405DAD8-BEE8-6F44-A10B-DD41FACE92E7}">
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="139" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="C26" zoomScale="139" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -10421,7 +10436,7 @@
       <c r="Y10" s="4"/>
       <c r="Z10" s="4"/>
     </row>
-    <row r="11" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="str">
         <f>IF(base!A11 &lt;&gt; "",base!A11, "")</f>
         <v>sexual_orientation</v>
@@ -10517,7 +10532,7 @@
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
     </row>
-    <row r="13" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="str">
         <f>IF(base!A13 &lt;&gt; "",base!A13, "")</f>
         <v>household_members</v>
@@ -10762,7 +10777,7 @@
       <c r="Y17" s="4"/>
       <c r="Z17" s="4"/>
     </row>
-    <row r="18" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="str">
         <f>IF(base!A18 &lt;&gt; "",base!A18, "")</f>
         <v>different_country_than_born_in</v>
@@ -10893,7 +10908,7 @@
       <c r="Y20" s="4"/>
       <c r="Z20" s="4"/>
     </row>
-    <row r="21" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="str">
         <f>IF(base!A21 &lt;&gt; "",base!A21, "")</f>
         <v>indoors_outdoors</v>
@@ -11105,7 +11120,7 @@
       <c r="Y24" s="4"/>
       <c r="Z24" s="4"/>
     </row>
-    <row r="25" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="str">
         <f>IF(base!A25 &lt;&gt; "",base!A25, "")</f>
         <v>environment_noise</v>
@@ -11179,7 +11194,7 @@
       </c>
       <c r="Z26" s="4"/>
     </row>
-    <row r="27" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="str">
         <f>IF(base!A27 &lt;&gt; "",base!A27, "")</f>
         <v>environment_lively</v>
@@ -11216,7 +11231,7 @@
       </c>
       <c r="Z27" s="4"/>
     </row>
-    <row r="28" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="str">
         <f>IF(base!A28 &lt;&gt; "",base!A28, "")</f>
         <v>environmen_pleasure</v>
@@ -11434,7 +11449,7 @@
       </c>
       <c r="Z33" s="4"/>
     </row>
-    <row r="34" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="str">
         <f>IF(base!A34 &lt;&gt; "",base!A34, "")</f>
         <v>sense_of_belonging</v>
@@ -11566,7 +11581,9 @@
       <c r="L36" s="3" t="s">
         <v>907</v>
       </c>
-      <c r="M36" s="3"/>
+      <c r="M36" s="3" t="s">
+        <v>942</v>
+      </c>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
@@ -11581,7 +11598,7 @@
       <c r="Y36" s="4"/>
       <c r="Z36" s="4"/>
     </row>
-    <row r="37" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="str">
         <f>IF(base!A37 &lt;&gt; "",base!A37, "")</f>
         <v>other_factors_negative</v>
@@ -11616,7 +11633,7 @@
       <c r="Y37" s="4"/>
       <c r="Z37" s="4"/>
     </row>
-    <row r="38" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="str">
         <f>IF(base!A38 &lt;&gt; "",base!A38, "")</f>
         <v>other_factors_positive</v>

</xml_diff>